<commit_message>
update definitions of some newly added terms
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@68680 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/Ontorat/20150630_newTerms.xlsx
+++ b/Load/src/ontology/Ontorat/20150630_newTerms.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
   <si>
     <t>Label</t>
   </si>
@@ -147,21 +147,6 @@
     <t>An average value for the number of clinical visits of a patient with malaria based on calendar years</t>
   </si>
   <si>
-    <t>Average number of anopheles (any species) that test positive for carrying Plasmodium parasites across all monthly light trap collection</t>
-  </si>
-  <si>
-    <t>Average number of anopheles (any species) that were tested for carrying Plasmodium parasites across all monthly light trap collection</t>
-  </si>
-  <si>
-    <t>Average percentage of anopheles (any species) that test positive for carrying Plasmodium parasites out of those tested. Averaged over all monthly light trap collections</t>
-  </si>
-  <si>
-    <t>Average number of anopheles (any species) collected across all monthly light trap collection</t>
-  </si>
-  <si>
-    <t>Total number of monthly light trap collections hat have been performed for the household of intrest</t>
-  </si>
-  <si>
     <t>number of anopheles (summed acrosss all species) collect from a single light trap collection</t>
   </si>
   <si>
@@ -172,6 +157,33 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBCS_0000170</t>
+  </si>
+  <si>
+    <t>average number of anopheles (any species) that test positive for carrying Plasmodium parasites across all monthly light trap collection</t>
+  </si>
+  <si>
+    <t>average number of anopheles (any species) that were tested for carrying Plasmodium parasites across all monthly light trap collection</t>
+  </si>
+  <si>
+    <t>average percentage of anopheles (any species) that test positive for carrying Plasmodium parasites out of those tested. Averaged over all monthly light trap collections</t>
+  </si>
+  <si>
+    <t>average number of anopheles (any species) collected across all monthly light trap collection</t>
+  </si>
+  <si>
+    <t>total number of monthly light trap collections hat have been performed for the household of intrest</t>
+  </si>
+  <si>
+    <t>average number of clinical visits where data was collected for a patient, average over calendar years</t>
+  </si>
+  <si>
+    <t>average number of clinical visits where data was collected for patient and the patient was diagnosed with asymptomatic parasitemia, average over calendar years</t>
+  </si>
+  <si>
+    <t>average number of clinical visits where data was collected for patient nd the patient was diagnosed with malaria, average over calendar years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A time datum for the duration of a patients participation in an investigation. </t>
   </si>
 </sst>
 </file>
@@ -671,7 +683,7 @@
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D2" sqref="D2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -721,11 +733,11 @@
       <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
-        <v>42</v>
+      <c r="E2" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>5</v>
@@ -747,11 +759,11 @@
       <c r="C3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E3" t="s">
-        <v>43</v>
+      <c r="E3" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>5</v>
@@ -773,11 +785,11 @@
       <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E4" t="s">
-        <v>44</v>
+      <c r="E4" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>5</v>
@@ -799,11 +811,11 @@
       <c r="C5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
-        <v>45</v>
+      <c r="E5" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>5</v>
@@ -825,11 +837,11 @@
       <c r="C6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E6" t="s">
-        <v>46</v>
+      <c r="E6" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>5</v>
@@ -849,13 +861,13 @@
         <v>26</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E7" t="s">
-        <v>47</v>
+      <c r="E7" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>5</v>
@@ -875,13 +887,13 @@
         <v>26</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E8" t="s">
-        <v>48</v>
+      <c r="E8" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>5</v>
@@ -901,13 +913,13 @@
         <v>26</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E9" t="s">
-        <v>49</v>
+      <c r="E9" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>5</v>
@@ -930,7 +942,7 @@
         <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
         <v>38</v>
@@ -959,7 +971,7 @@
         <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>5</v>
@@ -985,7 +997,7 @@
         <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>5</v>
@@ -1011,7 +1023,7 @@
         <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>5</v>

</xml_diff>